<commit_message>
Fixed typo and added comments about the to_date option
</commit_message>
<xml_diff>
--- a/tests/outputs/recent-collabs/coa_table.xlsx
+++ b/tests/outputs/recent-collabs/coa_table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12432" windowWidth="28800" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="NSF COA Template" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+    <numFmt formatCode="m/d/yy;@" numFmtId="164"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -260,206 +260,206 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="58">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyProtection="1" borderId="2" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyProtection="1" borderId="3" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyProtection="1" borderId="4" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyProtection="1" borderId="4" fillId="0" fontId="3" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyProtection="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyProtection="1" borderId="0" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" applyProtection="1" borderId="5" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" applyProtection="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" applyProtection="1" borderId="6" fillId="0" fontId="2" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" applyProtection="1" borderId="5" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" applyProtection="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" applyProtection="1" borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" applyProtection="1" borderId="8" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" applyProtection="1" borderId="8" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" applyProtection="1" borderId="9" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" applyProtection="1" borderId="1" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" applyProtection="1" borderId="6" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" applyProtection="1" borderId="7" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" applyProtection="1" borderId="9" fillId="0" fontId="2" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" applyProtection="1" borderId="6" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" applyProtection="1" borderId="6" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" applyProtection="1" borderId="5" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" applyProtection="1" borderId="1" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" applyProtection="1" borderId="1" fillId="0" fontId="13" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="6" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" applyProtection="1" borderId="6" fillId="0" fontId="12" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" applyProtection="1" borderId="8" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="7" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="2" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" indent="2" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection hidden="0" locked="0"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
   </cellStyles>
   <dxfs count="44">
     <dxf>
@@ -491,7 +491,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
       <font>
@@ -522,7 +522,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
       <font>
@@ -553,7 +553,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
       <font>
@@ -582,7 +582,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
       <border>
@@ -626,7 +626,7 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top"/>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
       <border>
@@ -670,19 +670,19 @@
           <color indexed="64"/>
         </horizontal>
       </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <sz val="10"/>
-        <vertAlign val="baseline"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+      <protection hidden="0" locked="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <sz val="10"/>
+        <vertAlign val="baseline"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt formatCode="m/d/yy;@" numFmtId="164"/>
       <alignment horizontal="general" vertical="top"/>
       <border outline="0">
         <left style="thin">
@@ -697,7 +697,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
       <font>
@@ -728,7 +728,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
       <font>
@@ -759,7 +759,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
       <font>
@@ -790,7 +790,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
       <font>
@@ -819,7 +819,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
       <border>
@@ -863,7 +863,7 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top"/>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
       <border>
@@ -907,19 +907,19 @@
           <color indexed="64"/>
         </horizontal>
       </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <sz val="10"/>
-        <vertAlign val="baseline"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+      <protection hidden="0" locked="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <sz val="10"/>
+        <vertAlign val="baseline"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt formatCode="m/d/yy;@" numFmtId="164"/>
       <alignment horizontal="general" vertical="top"/>
       <border>
         <left style="thin">
@@ -936,7 +936,7 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
       <font>
@@ -969,7 +969,7 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1002,7 +1002,7 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1035,7 +1035,7 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1066,7 +1066,7 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
       <border>
@@ -1126,19 +1126,19 @@
         <bottom/>
         <diagonal/>
       </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <sz val="10"/>
-        <vertAlign val="baseline"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+      <protection hidden="0" locked="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <sz val="10"/>
+        <vertAlign val="baseline"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt formatCode="m/d/yy;@" numFmtId="164"/>
       <alignment horizontal="general" vertical="top"/>
       <border outline="0">
         <left style="thin">
@@ -1153,7 +1153,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1184,7 +1184,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1215,7 +1215,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1246,7 +1246,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1275,7 +1275,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
       <border>
@@ -1319,7 +1319,7 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top"/>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
       <border>
@@ -1363,7 +1363,7 @@
           <color indexed="64"/>
         </horizontal>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection hidden="0" locked="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1394,7 +1394,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection locked="1" hidden="0"/>
+      <protection hidden="0" locked="1"/>
     </dxf>
     <dxf>
       <font>
@@ -1425,7 +1425,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection locked="1" hidden="0"/>
+      <protection hidden="0" locked="1"/>
     </dxf>
     <dxf>
       <font>
@@ -1456,7 +1456,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection locked="1" hidden="0"/>
+      <protection hidden="0" locked="1"/>
     </dxf>
     <dxf>
       <font>
@@ -1487,7 +1487,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection locked="1" hidden="0"/>
+      <protection hidden="0" locked="1"/>
     </dxf>
     <dxf>
       <font>
@@ -1503,89 +1503,89 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <sz val="10"/>
-        <vertAlign val="baseline"/>
-        <scheme val="minor"/>
-      </font>
-      <protection locked="1" hidden="0"/>
+      <protection hidden="0" locked="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <sz val="10"/>
+        <vertAlign val="baseline"/>
+        <scheme val="minor"/>
+      </font>
+      <protection hidden="0" locked="1"/>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TableA" displayName="TableA" ref="A16:D21" headerRowCount="1" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="42" displayName="TableA" headerRowCount="1" headerRowDxfId="43" id="1" name="TableA" ref="A16:D21" totalsRowShown="0">
   <tableColumns count="4">
-    <tableColumn id="1" name="1" dataDxfId="41"/>
-    <tableColumn id="2" name="Your Name:" dataDxfId="40"/>
-    <tableColumn id="3" name="Your Organizational Affiliation(s), last 12 mo" dataDxfId="39"/>
-    <tableColumn id="4" name="Last Active Date" dataDxfId="38"/>
+    <tableColumn dataDxfId="41" id="1" name="1"/>
+    <tableColumn dataDxfId="40" id="2" name="Your Name:"/>
+    <tableColumn dataDxfId="39" id="3" name="Your Organizational Affiliation(s), last 12 mo"/>
+    <tableColumn dataDxfId="38" id="4" name="Last Active Date"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight9" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TableD23" displayName="TableD23" ref="A26:E31" headerRowCount="1" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="35" displayName="TableD23" headerRowBorderDxfId="36" headerRowCount="1" headerRowDxfId="37" id="2" name="TableD23" ref="A26:E31" tableBorderDxfId="34" totalsRowBorderDxfId="33" totalsRowShown="0">
   <autoFilter ref="A26:E31"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="2" dataDxfId="32"/>
-    <tableColumn id="2" name="Name:" dataDxfId="31"/>
-    <tableColumn id="3" name="Type of Relationship" dataDxfId="30"/>
-    <tableColumn id="4" name="Optional  (email, Department)" dataDxfId="29" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" name="Last Active" dataDxfId="28"/>
+    <tableColumn dataDxfId="32" id="1" name="2"/>
+    <tableColumn dataDxfId="31" id="2" name="Name:"/>
+    <tableColumn dataDxfId="30" id="3" name="Type of Relationship"/>
+    <tableColumn dataCellStyle="Hyperlink" dataDxfId="29" id="4" name="Optional  (email, Department)"/>
+    <tableColumn dataDxfId="28" id="5" name="Last Active"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight9" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableD" displayName="TableD" ref="A50:E55" headerRowCount="1" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="TableD" headerRowBorderDxfId="26" headerRowCount="1" headerRowDxfId="27" id="3" name="TableD" ref="A50:E55" tableBorderDxfId="25" totalsRowBorderDxfId="24" totalsRowShown="0">
   <autoFilter ref="A50:E55"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="4" dataDxfId="23"/>
-    <tableColumn id="2" name="Name:" dataDxfId="22"/>
-    <tableColumn id="3" name="Organizational Affiliation" dataDxfId="21"/>
-    <tableColumn id="4" name="Optional  (email, Department)" dataDxfId="20" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" name="Last Active" dataDxfId="19"/>
+    <tableColumn dataDxfId="23" id="1" name="4"/>
+    <tableColumn dataDxfId="22" id="2" name="Name:"/>
+    <tableColumn dataDxfId="21" id="3" name="Organizational Affiliation"/>
+    <tableColumn dataCellStyle="Hyperlink" dataDxfId="20" id="4" name="Optional  (email, Department)"/>
+    <tableColumn dataDxfId="19" id="5" name="Last Active"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight9" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TableD5" displayName="TableD5" ref="A61:E66" headerRowCount="1" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="16" displayName="TableD5" headerRowBorderDxfId="17" headerRowCount="1" headerRowDxfId="18" id="4" name="TableD5" ref="A61:E66" tableBorderDxfId="15" totalsRowBorderDxfId="14" totalsRowShown="0">
   <autoFilter ref="A61:E66"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="5" dataDxfId="13"/>
-    <tableColumn id="2" name="Name:" dataDxfId="12"/>
-    <tableColumn id="3" name="Organizational Affiliation" dataDxfId="11"/>
-    <tableColumn id="4" name="Journal/Collection" dataDxfId="10" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" name="Last Active" dataDxfId="9"/>
+    <tableColumn dataDxfId="13" id="1" name="5"/>
+    <tableColumn dataDxfId="12" id="2" name="Name:"/>
+    <tableColumn dataDxfId="11" id="3" name="Organizational Affiliation"/>
+    <tableColumn dataCellStyle="Hyperlink" dataDxfId="10" id="4" name="Journal/Collection"/>
+    <tableColumn dataDxfId="9" id="5" name="Last Active"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight9" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TableC" displayName="TableC" ref="A37:D44" headerRowCount="1" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="6" displayName="TableC" headerRowBorderDxfId="7" headerRowCount="1" headerRowDxfId="8" id="5" name="TableC" ref="A37:D44" tableBorderDxfId="5" totalsRowBorderDxfId="4" totalsRowShown="0">
   <autoFilter ref="A37:D44"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="3" dataDxfId="3"/>
-    <tableColumn id="2" name="Advisor/Advisee Name:" dataDxfId="2"/>
-    <tableColumn id="3" name="Organizational Affiliation" dataDxfId="1"/>
-    <tableColumn id="4" name="Optional  (email, Department)" dataDxfId="0" dataCellStyle="Hyperlink"/>
+    <tableColumn dataDxfId="3" id="1" name="3"/>
+    <tableColumn dataDxfId="2" id="2" name="Advisor/Advisee Name:"/>
+    <tableColumn dataDxfId="1" id="3" name="Organizational Affiliation"/>
+    <tableColumn dataCellStyle="Hyperlink" dataDxfId="0" id="4" name="Optional  (email, Department)"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight9" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
 </table>
 </file>
 
@@ -1798,25 +1798,25 @@
   </sheetPr>
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="145" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="145" zoomScaleSheetLayoutView="100">
       <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="0" defaultRowHeight="13.8"/>
   <cols>
-    <col width="4.33203125" customWidth="1" style="9" min="1" max="1"/>
-    <col width="22.33203125" customWidth="1" style="9" min="2" max="2"/>
-    <col width="34.5546875" customWidth="1" style="9" min="3" max="3"/>
-    <col width="29.33203125" customWidth="1" style="9" min="4" max="4"/>
-    <col width="12.44140625" customWidth="1" style="9" min="5" max="5"/>
-    <col width="2.5546875" customWidth="1" style="9" min="6" max="6"/>
-    <col hidden="1" style="9" min="7" max="17"/>
-    <col hidden="1" width="2.33203125" customWidth="1" style="9" min="18" max="18"/>
-    <col hidden="1" style="9" min="19" max="19"/>
-    <col hidden="1" style="9" min="20" max="16384"/>
+    <col customWidth="1" max="1" min="1" style="9" width="4.33203125"/>
+    <col customWidth="1" max="2" min="2" style="9" width="22.33203125"/>
+    <col customWidth="1" max="3" min="3" style="9" width="34.5546875"/>
+    <col customWidth="1" max="4" min="4" style="9" width="29.33203125"/>
+    <col customWidth="1" max="5" min="5" style="9" width="12.44140625"/>
+    <col customWidth="1" max="6" min="6" style="9" width="2.5546875"/>
+    <col hidden="1" max="17" min="7" style="9"/>
+    <col customWidth="1" hidden="1" max="18" min="18" style="9" width="2.33203125"/>
+    <col hidden="1" max="19" min="19" style="9"/>
+    <col hidden="1" max="16384" min="20" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" ht="195.6" customHeight="1" s="49">
+    <row customHeight="1" ht="195.6" r="1" s="49">
       <c r="A1" s="50" t="inlineStr">
         <is>
           <t xml:space="preserve">The following information regarding collaborators and other affiliations (COA) must be separately provided for each individual identified as senior project personnel.  The COA information must be provided through use of this COA template.  
@@ -1825,7 +1825,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="99" customFormat="1" customHeight="1" s="9">
+    <row customFormat="1" customHeight="1" ht="99" r="2" s="9">
       <c r="A2" s="55" t="inlineStr">
         <is>
           <t xml:space="preserve">There are five separate categories of information which correspond to the five tables in the COA template:
@@ -1834,7 +1834,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="67.34999999999999" customFormat="1" customHeight="1" s="9">
+    <row customFormat="1" customHeight="1" ht="67.34999999999999" r="3" s="9">
       <c r="A3" s="55" t="inlineStr">
         <is>
           <t>COA template Table 2:
@@ -1842,7 +1842,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="72.59999999999999" customFormat="1" customHeight="1" s="9">
+    <row customFormat="1" customHeight="1" ht="72.59999999999999" r="4" s="9">
       <c r="A4" s="55" t="inlineStr">
         <is>
           <t>COA template Table 3:
@@ -1852,7 +1852,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="74.25" customFormat="1" customHeight="1" s="9">
+    <row customFormat="1" customHeight="1" ht="74.25" r="5" s="9">
       <c r="A5" s="55" t="inlineStr">
         <is>
           <t xml:space="preserve">COA template Table 4:
@@ -1863,7 +1863,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="76.5" customFormat="1" customHeight="1" s="9">
+    <row customFormat="1" customHeight="1" ht="76.5" r="6" s="9">
       <c r="A6" s="55" t="inlineStr">
         <is>
           <t>COA template Table 5:
@@ -1873,7 +1873,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="113.25" customFormat="1" customHeight="1" s="10">
+    <row customFormat="1" customHeight="1" ht="113.25" r="7" s="10">
       <c r="A7" s="52" t="inlineStr">
         <is>
           <t xml:space="preserve">The template has been developed to be fillable, however, the content and format requirements must not be altered by the user.  This template must be saved in .xlsx or .xls format, and directly uploaded into FastLane as a Collaborators and Other Affiliations Single Copy Document.  Using the .xlsx or .xls format will enable preservation of searchable text that otherwise would be lost.  It is therefore imperative that this document be uploaded in .xlsx or .xls only.  Uploading a document in any format other than .xlsx or .xls may delay the timely processing and review of the proposal.
@@ -1881,7 +1881,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="62.7" customHeight="1" s="49">
+    <row customHeight="1" ht="62.7" r="8" s="49">
       <c r="A8" s="52" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1 Note that graduate advisors are no longer required to be reported.
@@ -1889,7 +1889,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="14.1" customHeight="1" s="49">
+    <row customHeight="1" ht="14.1" r="9" s="49">
       <c r="A9" s="52" t="inlineStr">
         <is>
           <t>List names as Last Name, First Name, Middle Initial.  Additionally, provide email, organization, and department (optional) to disambiguate common names.</t>
@@ -1910,7 +1910,7 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="15.45" customFormat="1" customHeight="1" s="9">
+    <row customFormat="1" customHeight="1" ht="15.45" r="12" s="9">
       <c r="A12" s="53" t="inlineStr">
         <is>
           <t xml:space="preserve">
@@ -1918,7 +1918,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="49.2" customFormat="1" customHeight="1" s="9">
+    <row customFormat="1" customHeight="1" ht="49.2" r="13" s="9">
       <c r="A13" s="52" t="inlineStr">
         <is>
           <t xml:space="preserve">For "Last Active Date" and "Last Active" columns dates are optional, but will help NSF staff easily determine which information remains relevant for reviewer selection. 
@@ -1926,8 +1926,8 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="12" customHeight="1" s="49"/>
-    <row r="15" ht="29.4" customHeight="1" s="49">
+    <row customHeight="1" ht="12" r="14" s="49"/>
+    <row customHeight="1" ht="29.4" r="15" s="49">
       <c r="A15" s="48" t="inlineStr">
         <is>
           <t>Table 1: List the individual’s last name, first name, middle initial, and organizational affiliation in the last 12 months.</t>
@@ -1957,7 +1957,7 @@
       </c>
       <c r="E16" s="4" t="n"/>
     </row>
-    <row r="17" customFormat="1" s="9">
+    <row customFormat="1" r="17" s="9">
       <c r="A17" s="43" t="n"/>
       <c r="B17" s="44" t="inlineStr">
         <is>
@@ -1972,7 +1972,7 @@
       <c r="D17" s="43" t="n"/>
       <c r="E17" s="4" t="n"/>
     </row>
-    <row r="18" customFormat="1" s="9">
+    <row customFormat="1" r="18" s="9">
       <c r="A18" s="43" t="n"/>
       <c r="B18" s="43" t="n"/>
       <c r="C18" s="44" t="inlineStr">
@@ -2005,7 +2005,7 @@
       <c r="D20" s="47" t="n"/>
       <c r="E20" s="4" t="n"/>
     </row>
-    <row r="21" ht="30.6" customFormat="1" customHeight="1" s="12">
+    <row customFormat="1" customHeight="1" ht="30.6" r="21" s="12">
       <c r="A21" s="43" t="n"/>
       <c r="B21" s="43" t="n"/>
       <c r="C21" s="46" t="n"/>
@@ -2015,14 +2015,14 @@
     <row r="22">
       <c r="E22" s="4" t="n"/>
     </row>
-    <row r="23" ht="28.95" customHeight="1" s="49">
+    <row customHeight="1" ht="28.95" r="23" s="49">
       <c r="A23" s="48" t="inlineStr">
         <is>
           <t>Table 2: List names as last name, first name, middle initial, for whom a personal, family, or business relationship would otherwise preclude their service as a reviewer.</t>
         </is>
       </c>
     </row>
-    <row r="24" customFormat="1" s="9">
+    <row customFormat="1" r="24" s="9">
       <c r="A24" s="56" t="inlineStr">
         <is>
           <t>R:</t>
@@ -2045,7 +2045,7 @@
       </c>
       <c r="E25" s="3" t="n"/>
     </row>
-    <row r="26" customFormat="1" s="9">
+    <row customFormat="1" r="26" s="9">
       <c r="A26" s="13" t="inlineStr">
         <is>
           <t>2</t>
@@ -2072,7 +2072,7 @@
         </is>
       </c>
     </row>
-    <row r="27" customFormat="1" s="9">
+    <row customFormat="1" r="27" s="9">
       <c r="A27" s="19" t="inlineStr">
         <is>
           <t>R:</t>
@@ -2091,42 +2091,42 @@
       <c r="D27" s="20" t="n"/>
       <c r="E27" s="21" t="n"/>
     </row>
-    <row r="28" customFormat="1" s="9">
+    <row customFormat="1" r="28" s="9">
       <c r="A28" s="22" t="n"/>
       <c r="B28" s="20" t="n"/>
       <c r="C28" s="23" t="n"/>
       <c r="D28" s="20" t="n"/>
       <c r="E28" s="21" t="n"/>
     </row>
-    <row r="29" customFormat="1" s="9">
+    <row customFormat="1" r="29" s="9">
       <c r="A29" s="34" t="n"/>
       <c r="B29" s="35" t="n"/>
       <c r="C29" s="35" t="n"/>
       <c r="D29" s="36" t="n"/>
       <c r="E29" s="37" t="n"/>
     </row>
-    <row r="30" customFormat="1" s="9">
+    <row customFormat="1" r="30" s="9">
       <c r="A30" s="34" t="n"/>
       <c r="B30" s="35" t="n"/>
       <c r="C30" s="35" t="n"/>
       <c r="D30" s="36" t="n"/>
       <c r="E30" s="37" t="n"/>
     </row>
-    <row r="31" customFormat="1" s="9">
+    <row customFormat="1" r="31" s="9">
       <c r="A31" s="34" t="n"/>
       <c r="B31" s="35" t="n"/>
       <c r="C31" s="35" t="n"/>
       <c r="D31" s="36" t="n"/>
       <c r="E31" s="37" t="n"/>
     </row>
-    <row r="32" ht="30.6" customFormat="1" customHeight="1" s="9">
+    <row customFormat="1" customHeight="1" ht="30.6" r="32" s="9">
       <c r="A32" s="17" t="n"/>
       <c r="B32" s="18" t="n"/>
       <c r="C32" s="18" t="n"/>
       <c r="D32" s="18" t="n"/>
       <c r="E32" s="4" t="n"/>
     </row>
-    <row r="33" ht="28.95" customFormat="1" customHeight="1" s="9">
+    <row customFormat="1" customHeight="1" ht="28.95" r="33" s="9">
       <c r="A33" s="48" t="inlineStr">
         <is>
           <t>Table 3: List names as last name, first name, middle initial, and provide organizational affiliations, if known, for the following.</t>
@@ -2222,51 +2222,51 @@
       <c r="C39" s="20" t="n"/>
       <c r="D39" s="33" t="n"/>
     </row>
-    <row r="40" customFormat="1" s="9">
+    <row customFormat="1" r="40" s="9">
       <c r="A40" s="19" t="n"/>
       <c r="B40" s="20" t="n"/>
       <c r="C40" s="20" t="n"/>
       <c r="D40" s="32" t="n"/>
     </row>
-    <row r="41" customFormat="1" s="9">
+    <row customFormat="1" r="41" s="9">
       <c r="A41" s="19" t="n"/>
       <c r="B41" s="20" t="n"/>
       <c r="C41" s="20" t="n"/>
       <c r="D41" s="32" t="n"/>
     </row>
-    <row r="42" customFormat="1" s="9">
+    <row customFormat="1" r="42" s="9">
       <c r="A42" s="19" t="n"/>
       <c r="B42" s="35" t="n"/>
       <c r="C42" s="35" t="n"/>
       <c r="D42" s="36" t="n"/>
     </row>
-    <row r="43" customFormat="1" s="9">
+    <row customFormat="1" r="43" s="9">
       <c r="A43" s="19" t="n"/>
       <c r="B43" s="35" t="n"/>
       <c r="C43" s="35" t="n"/>
       <c r="D43" s="36" t="n"/>
     </row>
-    <row r="44" customFormat="1" s="9">
+    <row customFormat="1" r="44" s="9">
       <c r="A44" s="19" t="n"/>
       <c r="B44" s="35" t="n"/>
       <c r="C44" s="35" t="n"/>
       <c r="D44" s="36" t="n"/>
     </row>
-    <row r="45" customFormat="1" s="56">
+    <row customFormat="1" r="45" s="56">
       <c r="A45" s="9" t="n"/>
       <c r="B45" s="9" t="n"/>
       <c r="C45" s="9" t="n"/>
       <c r="D45" s="9" t="n"/>
       <c r="E45" s="4" t="n"/>
     </row>
-    <row r="46" ht="28.35" customFormat="1" customHeight="1" s="56">
+    <row customFormat="1" customHeight="1" ht="28.35" r="46" s="56">
       <c r="A46" s="48" t="inlineStr">
         <is>
           <t>Table 4: List names as last name, first name, middle initial, and provide organizational affiliations, if known, for the following:</t>
         </is>
       </c>
     </row>
-    <row r="47" ht="27" customFormat="1" customHeight="1" s="56">
+    <row customFormat="1" customHeight="1" ht="27" r="47" s="56">
       <c r="A47" s="11" t="inlineStr">
         <is>
           <t>A:</t>
@@ -2304,7 +2304,7 @@
       </c>
       <c r="E49" s="3" t="n"/>
     </row>
-    <row r="50" customFormat="1" s="9">
+    <row customFormat="1" r="50" s="9">
       <c r="A50" s="13" t="inlineStr">
         <is>
           <t>4</t>
@@ -2331,7 +2331,7 @@
         </is>
       </c>
     </row>
-    <row r="51" customFormat="1" s="9">
+    <row customFormat="1" r="51" s="9">
       <c r="A51" s="57" t="inlineStr">
         <is>
           <t>A:</t>
@@ -2350,28 +2350,28 @@
       <c r="D51" s="57" t="n"/>
       <c r="E51" s="57" t="n"/>
     </row>
-    <row r="52" customFormat="1" s="9">
+    <row customFormat="1" r="52" s="9">
       <c r="A52" s="30" t="n"/>
       <c r="B52" s="39" t="n"/>
       <c r="C52" s="39" t="n"/>
       <c r="D52" s="39" t="n"/>
       <c r="E52" s="31" t="n"/>
     </row>
-    <row r="53" customFormat="1" s="9">
+    <row customFormat="1" r="53" s="9">
       <c r="A53" s="9" t="n"/>
       <c r="B53" s="9" t="n"/>
       <c r="C53" s="9" t="n"/>
       <c r="D53" s="9" t="n"/>
       <c r="E53" s="9" t="n"/>
     </row>
-    <row r="54" customFormat="1" s="9">
+    <row customFormat="1" r="54" s="9">
       <c r="A54" s="48" t="inlineStr">
         <is>
           <t>Table 5: List editorial board, editor-in chief and co-editors with whom the individual interacts.  An editor-in-chief must list the entire editorial board.</t>
         </is>
       </c>
     </row>
-    <row r="55" customFormat="1" s="9">
+    <row customFormat="1" r="55" s="9">
       <c r="A55" s="56" t="inlineStr">
         <is>
           <t>B:</t>
@@ -2384,7 +2384,7 @@
       </c>
       <c r="E55" s="3" t="n"/>
     </row>
-    <row r="56" ht="16.95" customFormat="1" customHeight="1" s="56">
+    <row customFormat="1" customHeight="1" ht="16.95" r="56" s="56">
       <c r="A56" s="56" t="inlineStr">
         <is>
           <t>E:</t>
@@ -2397,7 +2397,7 @@
       </c>
       <c r="E56" s="3" t="n"/>
     </row>
-    <row r="57" ht="28.95" customFormat="1" customHeight="1" s="56">
+    <row customFormat="1" customHeight="1" ht="28.95" r="57" s="56">
       <c r="A57" s="56" t="n"/>
       <c r="B57" s="56" t="n"/>
       <c r="C57" s="56" t="n"/>
@@ -2408,7 +2408,7 @@
       </c>
       <c r="E57" s="3" t="n"/>
     </row>
-    <row r="58" customFormat="1" s="56">
+    <row customFormat="1" r="58" s="56">
       <c r="A58" s="13" t="inlineStr">
         <is>
           <t>5</t>
@@ -2435,7 +2435,7 @@
         </is>
       </c>
     </row>
-    <row r="59" customFormat="1" s="56">
+    <row customFormat="1" r="59" s="56">
       <c r="A59" s="19" t="inlineStr">
         <is>
           <t>B:</t>
@@ -2460,7 +2460,7 @@
         <v>42736</v>
       </c>
     </row>
-    <row r="60" customFormat="1" s="9">
+    <row customFormat="1" r="60" s="9">
       <c r="A60" s="22" t="inlineStr">
         <is>
           <t>E:</t>
@@ -2471,28 +2471,28 @@
       <c r="D60" s="20" t="n"/>
       <c r="E60" s="21" t="n"/>
     </row>
-    <row r="61" customFormat="1" s="9">
+    <row customFormat="1" r="61" s="9">
       <c r="A61" s="22" t="n"/>
       <c r="B61" s="23" t="n"/>
       <c r="C61" s="23" t="n"/>
       <c r="D61" s="28" t="n"/>
       <c r="E61" s="21" t="n"/>
     </row>
-    <row r="62" customFormat="1" s="9">
+    <row customFormat="1" r="62" s="9">
       <c r="A62" s="22" t="n"/>
       <c r="B62" s="23" t="n"/>
       <c r="C62" s="23" t="n"/>
       <c r="D62" s="28" t="n"/>
       <c r="E62" s="21" t="n"/>
     </row>
-    <row r="63" customFormat="1" s="9">
+    <row customFormat="1" r="63" s="9">
       <c r="A63" s="24" t="n"/>
       <c r="B63" s="25" t="n"/>
       <c r="C63" s="25" t="n"/>
       <c r="D63" s="26" t="n"/>
       <c r="E63" s="27" t="n"/>
     </row>
-    <row r="64" customFormat="1" s="9"/>
+    <row customFormat="1" r="64" s="9"/>
     <row r="65"/>
     <row r="66"/>
   </sheetData>
@@ -2521,27 +2521,27 @@
     <mergeCell ref="B24:E24"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation sqref="A51:A55" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="A51:A55" type="list">
       <formula1>"A:,C:"</formula1>
     </dataValidation>
-    <dataValidation sqref="A27:A31" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="A27:A31" type="list">
       <formula1>"R:"</formula1>
     </dataValidation>
-    <dataValidation sqref="A32" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="A32" type="list">
       <formula1>"G:,T:,P:"</formula1>
     </dataValidation>
-    <dataValidation sqref="A62:A66" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="A62:A66" type="list">
       <formula1>"B:,E:"</formula1>
     </dataValidation>
-    <dataValidation sqref="A38:A44" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="A38:A44" type="list">
       <formula1>"G:,T:"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1" display="https://www.nsf.gov/bfa/dias/policy/coa.jsp" r:id="rId1"/>
+    <hyperlink display="https://www.nsf.gov/bfa/dias/policy/coa.jsp" ref="A1" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" scale="98" fitToHeight="0"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" orientation="portrait" scale="98"/>
   <tableParts count="5">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>

</xml_diff>

<commit_message>
Added options to test for the recent-collabs builder (comparing excel files). Test passed for now."
</commit_message>
<xml_diff>
--- a/tests/outputs/recent-collabs/coa_table.xlsx
+++ b/tests/outputs/recent-collabs/coa_table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12432" windowWidth="28800" xWindow="0" yWindow="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="NSF COA Template" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="m/d/yy;@" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -260,206 +260,206 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="58">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyProtection="1" borderId="2" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyProtection="1" borderId="3" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyProtection="1" borderId="4" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyProtection="1" borderId="4" fillId="0" fontId="3" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="5" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="6" fillId="0" fontId="2" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="5" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="8" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="8" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="top"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="9" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="1" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="top"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="6" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="7" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="9" fillId="0" fontId="2" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="6" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="6" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="top"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="5" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="1" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="1" fillId="0" fontId="13" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="top"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="6" fillId="0" fontId="12" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="6" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="8" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="3" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="7" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" indent="2" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" indent="2" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection hidden="0" locked="0"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="44">
     <dxf>
@@ -491,7 +491,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -522,7 +522,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -553,7 +553,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -582,7 +582,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <border>
@@ -626,7 +626,7 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top"/>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <border>
@@ -670,19 +670,19 @@
           <color indexed="64"/>
         </horizontal>
       </border>
-      <protection hidden="0" locked="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <sz val="10"/>
-        <vertAlign val="baseline"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt formatCode="m/d/yy;@" numFmtId="164"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <sz val="10"/>
+        <vertAlign val="baseline"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
       <alignment horizontal="general" vertical="top"/>
       <border outline="0">
         <left style="thin">
@@ -697,7 +697,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -728,7 +728,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -759,7 +759,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -790,7 +790,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -819,7 +819,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <border>
@@ -863,7 +863,7 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top"/>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <border>
@@ -907,19 +907,19 @@
           <color indexed="64"/>
         </horizontal>
       </border>
-      <protection hidden="0" locked="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <sz val="10"/>
-        <vertAlign val="baseline"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt formatCode="m/d/yy;@" numFmtId="164"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <sz val="10"/>
+        <vertAlign val="baseline"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
       <alignment horizontal="general" vertical="top"/>
       <border>
         <left style="thin">
@@ -936,7 +936,7 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -969,7 +969,7 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1002,7 +1002,7 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1035,7 +1035,7 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1066,7 +1066,7 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <border>
@@ -1126,19 +1126,19 @@
         <bottom/>
         <diagonal/>
       </border>
-      <protection hidden="0" locked="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <sz val="10"/>
-        <vertAlign val="baseline"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt formatCode="m/d/yy;@" numFmtId="164"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <sz val="10"/>
+        <vertAlign val="baseline"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
       <alignment horizontal="general" vertical="top"/>
       <border outline="0">
         <left style="thin">
@@ -1153,7 +1153,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1184,7 +1184,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1215,7 +1215,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1246,7 +1246,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1275,7 +1275,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <border>
@@ -1319,7 +1319,7 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top"/>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <border>
@@ -1363,7 +1363,7 @@
           <color indexed="64"/>
         </horizontal>
       </border>
-      <protection hidden="0" locked="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1394,7 +1394,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection hidden="0" locked="1"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1425,7 +1425,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection hidden="0" locked="1"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1456,7 +1456,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection hidden="0" locked="1"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1487,7 +1487,7 @@
         </bottom>
         <diagonal/>
       </border>
-      <protection hidden="0" locked="1"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1503,89 +1503,89 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top"/>
-      <protection hidden="0" locked="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Calibri"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <sz val="10"/>
-        <vertAlign val="baseline"/>
-        <scheme val="minor"/>
-      </font>
-      <protection hidden="0" locked="1"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <sz val="10"/>
+        <vertAlign val="baseline"/>
+        <scheme val="minor"/>
+      </font>
+      <protection locked="1" hidden="0"/>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="42" displayName="TableA" headerRowCount="1" headerRowDxfId="43" id="1" name="TableA" ref="A16:D21" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TableA" displayName="TableA" ref="A16:D21" headerRowCount="1" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <tableColumns count="4">
-    <tableColumn dataDxfId="41" id="1" name="1"/>
-    <tableColumn dataDxfId="40" id="2" name="Your Name:"/>
-    <tableColumn dataDxfId="39" id="3" name="Your Organizational Affiliation(s), last 12 mo"/>
-    <tableColumn dataDxfId="38" id="4" name="Last Active Date"/>
+    <tableColumn id="1" name="1" dataDxfId="41"/>
+    <tableColumn id="2" name="Your Name:" dataDxfId="40"/>
+    <tableColumn id="3" name="Your Organizational Affiliation(s), last 12 mo" dataDxfId="39"/>
+    <tableColumn id="4" name="Last Active Date" dataDxfId="38"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="35" displayName="TableD23" headerRowBorderDxfId="36" headerRowCount="1" headerRowDxfId="37" id="2" name="TableD23" ref="A26:E31" tableBorderDxfId="34" totalsRowBorderDxfId="33" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TableD23" displayName="TableD23" ref="A26:E31" headerRowCount="1" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <autoFilter ref="A26:E31"/>
   <tableColumns count="5">
-    <tableColumn dataDxfId="32" id="1" name="2"/>
-    <tableColumn dataDxfId="31" id="2" name="Name:"/>
-    <tableColumn dataDxfId="30" id="3" name="Type of Relationship"/>
-    <tableColumn dataCellStyle="Hyperlink" dataDxfId="29" id="4" name="Optional  (email, Department)"/>
-    <tableColumn dataDxfId="28" id="5" name="Last Active"/>
+    <tableColumn id="1" name="2" dataDxfId="32"/>
+    <tableColumn id="2" name="Name:" dataDxfId="31"/>
+    <tableColumn id="3" name="Type of Relationship" dataDxfId="30"/>
+    <tableColumn id="4" name="Optional  (email, Department)" dataDxfId="29" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" name="Last Active" dataDxfId="28"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" displayName="TableD" headerRowBorderDxfId="26" headerRowCount="1" headerRowDxfId="27" id="3" name="TableD" ref="A50:E55" tableBorderDxfId="25" totalsRowBorderDxfId="24" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="TableD" displayName="TableD" ref="A50:E55" headerRowCount="1" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
   <autoFilter ref="A50:E55"/>
   <tableColumns count="5">
-    <tableColumn dataDxfId="23" id="1" name="4"/>
-    <tableColumn dataDxfId="22" id="2" name="Name:"/>
-    <tableColumn dataDxfId="21" id="3" name="Organizational Affiliation"/>
-    <tableColumn dataCellStyle="Hyperlink" dataDxfId="20" id="4" name="Optional  (email, Department)"/>
-    <tableColumn dataDxfId="19" id="5" name="Last Active"/>
+    <tableColumn id="1" name="4" dataDxfId="23"/>
+    <tableColumn id="2" name="Name:" dataDxfId="22"/>
+    <tableColumn id="3" name="Organizational Affiliation" dataDxfId="21"/>
+    <tableColumn id="4" name="Optional  (email, Department)" dataDxfId="20" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" name="Last Active" dataDxfId="19"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="16" displayName="TableD5" headerRowBorderDxfId="17" headerRowCount="1" headerRowDxfId="18" id="4" name="TableD5" ref="A61:E66" tableBorderDxfId="15" totalsRowBorderDxfId="14" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TableD5" displayName="TableD5" ref="A61:E66" headerRowCount="1" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="A61:E66"/>
   <tableColumns count="5">
-    <tableColumn dataDxfId="13" id="1" name="5"/>
-    <tableColumn dataDxfId="12" id="2" name="Name:"/>
-    <tableColumn dataDxfId="11" id="3" name="Organizational Affiliation"/>
-    <tableColumn dataCellStyle="Hyperlink" dataDxfId="10" id="4" name="Journal/Collection"/>
-    <tableColumn dataDxfId="9" id="5" name="Last Active"/>
+    <tableColumn id="1" name="5" dataDxfId="13"/>
+    <tableColumn id="2" name="Name:" dataDxfId="12"/>
+    <tableColumn id="3" name="Organizational Affiliation" dataDxfId="11"/>
+    <tableColumn id="4" name="Journal/Collection" dataDxfId="10" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" name="Last Active" dataDxfId="9"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" dataDxfId="6" displayName="TableC" headerRowBorderDxfId="7" headerRowCount="1" headerRowDxfId="8" id="5" name="TableC" ref="A37:D44" tableBorderDxfId="5" totalsRowBorderDxfId="4" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TableC" displayName="TableC" ref="A37:D44" headerRowCount="1" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="A37:D44"/>
   <tableColumns count="4">
-    <tableColumn dataDxfId="3" id="1" name="3"/>
-    <tableColumn dataDxfId="2" id="2" name="Advisor/Advisee Name:"/>
-    <tableColumn dataDxfId="1" id="3" name="Organizational Affiliation"/>
-    <tableColumn dataCellStyle="Hyperlink" dataDxfId="0" id="4" name="Optional  (email, Department)"/>
+    <tableColumn id="1" name="3" dataDxfId="3"/>
+    <tableColumn id="2" name="Advisor/Advisee Name:" dataDxfId="2"/>
+    <tableColumn id="3" name="Organizational Affiliation" dataDxfId="1"/>
+    <tableColumn id="4" name="Optional  (email, Department)" dataDxfId="0" dataCellStyle="Hyperlink"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showColumnStripes="0" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1798,25 +1798,25 @@
   </sheetPr>
   <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="145" zoomScaleSheetLayoutView="100">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="145" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="0" defaultRowHeight="13.8"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="9" width="4.33203125"/>
-    <col customWidth="1" max="2" min="2" style="9" width="22.33203125"/>
-    <col customWidth="1" max="3" min="3" style="9" width="34.5546875"/>
-    <col customWidth="1" max="4" min="4" style="9" width="29.33203125"/>
-    <col customWidth="1" max="5" min="5" style="9" width="12.44140625"/>
-    <col customWidth="1" max="6" min="6" style="9" width="2.5546875"/>
-    <col hidden="1" max="17" min="7" style="9"/>
-    <col customWidth="1" hidden="1" max="18" min="18" style="9" width="2.33203125"/>
-    <col hidden="1" max="19" min="19" style="9"/>
-    <col hidden="1" max="16384" min="20" style="9"/>
+    <col width="4.33203125" customWidth="1" style="9" min="1" max="1"/>
+    <col width="22.33203125" customWidth="1" style="9" min="2" max="2"/>
+    <col width="34.5546875" customWidth="1" style="9" min="3" max="3"/>
+    <col width="29.33203125" customWidth="1" style="9" min="4" max="4"/>
+    <col width="12.44140625" customWidth="1" style="9" min="5" max="5"/>
+    <col width="2.5546875" customWidth="1" style="9" min="6" max="6"/>
+    <col hidden="1" style="9" min="7" max="17"/>
+    <col hidden="1" width="2.33203125" customWidth="1" style="9" min="18" max="18"/>
+    <col hidden="1" style="9" min="19" max="19"/>
+    <col hidden="1" style="9" min="20" max="16384"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="195.6" r="1" s="49">
+    <row r="1" ht="195.6" customHeight="1" s="49">
       <c r="A1" s="50" t="inlineStr">
         <is>
           <t xml:space="preserve">The following information regarding collaborators and other affiliations (COA) must be separately provided for each individual identified as senior project personnel.  The COA information must be provided through use of this COA template.  
@@ -1825,7 +1825,7 @@
         </is>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="99" r="2" s="9">
+    <row r="2" ht="99" customFormat="1" customHeight="1" s="9">
       <c r="A2" s="55" t="inlineStr">
         <is>
           <t xml:space="preserve">There are five separate categories of information which correspond to the five tables in the COA template:
@@ -1834,7 +1834,7 @@
         </is>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="67.34999999999999" r="3" s="9">
+    <row r="3" ht="67.34999999999999" customFormat="1" customHeight="1" s="9">
       <c r="A3" s="55" t="inlineStr">
         <is>
           <t>COA template Table 2:
@@ -1842,7 +1842,7 @@
         </is>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="72.59999999999999" r="4" s="9">
+    <row r="4" ht="72.59999999999999" customFormat="1" customHeight="1" s="9">
       <c r="A4" s="55" t="inlineStr">
         <is>
           <t>COA template Table 3:
@@ -1852,7 +1852,7 @@
         </is>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="74.25" r="5" s="9">
+    <row r="5" ht="74.25" customFormat="1" customHeight="1" s="9">
       <c r="A5" s="55" t="inlineStr">
         <is>
           <t xml:space="preserve">COA template Table 4:
@@ -1863,7 +1863,7 @@
         </is>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="76.5" r="6" s="9">
+    <row r="6" ht="76.5" customFormat="1" customHeight="1" s="9">
       <c r="A6" s="55" t="inlineStr">
         <is>
           <t>COA template Table 5:
@@ -1873,7 +1873,7 @@
         </is>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="113.25" r="7" s="10">
+    <row r="7" ht="113.25" customFormat="1" customHeight="1" s="10">
       <c r="A7" s="52" t="inlineStr">
         <is>
           <t xml:space="preserve">The template has been developed to be fillable, however, the content and format requirements must not be altered by the user.  This template must be saved in .xlsx or .xls format, and directly uploaded into FastLane as a Collaborators and Other Affiliations Single Copy Document.  Using the .xlsx or .xls format will enable preservation of searchable text that otherwise would be lost.  It is therefore imperative that this document be uploaded in .xlsx or .xls only.  Uploading a document in any format other than .xlsx or .xls may delay the timely processing and review of the proposal.
@@ -1881,7 +1881,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="62.7" r="8" s="49">
+    <row r="8" ht="62.7" customHeight="1" s="49">
       <c r="A8" s="52" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1 Note that graduate advisors are no longer required to be reported.
@@ -1889,7 +1889,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="14.1" r="9" s="49">
+    <row r="9" ht="14.1" customHeight="1" s="49">
       <c r="A9" s="52" t="inlineStr">
         <is>
           <t>List names as Last Name, First Name, Middle Initial.  Additionally, provide email, organization, and department (optional) to disambiguate common names.</t>
@@ -1910,7 +1910,7 @@
         </is>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.45" r="12" s="9">
+    <row r="12" ht="15.45" customFormat="1" customHeight="1" s="9">
       <c r="A12" s="53" t="inlineStr">
         <is>
           <t xml:space="preserve">
@@ -1918,7 +1918,7 @@
         </is>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="49.2" r="13" s="9">
+    <row r="13" ht="49.2" customFormat="1" customHeight="1" s="9">
       <c r="A13" s="52" t="inlineStr">
         <is>
           <t xml:space="preserve">For "Last Active Date" and "Last Active" columns dates are optional, but will help NSF staff easily determine which information remains relevant for reviewer selection. 
@@ -1926,8 +1926,8 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="12" r="14" s="49"/>
-    <row customHeight="1" ht="29.4" r="15" s="49">
+    <row r="14" ht="12" customHeight="1" s="49"/>
+    <row r="15" ht="29.4" customHeight="1" s="49">
       <c r="A15" s="48" t="inlineStr">
         <is>
           <t>Table 1: List the individual’s last name, first name, middle initial, and organizational affiliation in the last 12 months.</t>
@@ -1957,7 +1957,7 @@
       </c>
       <c r="E16" s="4" t="n"/>
     </row>
-    <row customFormat="1" r="17" s="9">
+    <row r="17" customFormat="1" s="9">
       <c r="A17" s="43" t="n"/>
       <c r="B17" s="44" t="inlineStr">
         <is>
@@ -1972,7 +1972,7 @@
       <c r="D17" s="43" t="n"/>
       <c r="E17" s="4" t="n"/>
     </row>
-    <row customFormat="1" r="18" s="9">
+    <row r="18" customFormat="1" s="9">
       <c r="A18" s="43" t="n"/>
       <c r="B18" s="43" t="n"/>
       <c r="C18" s="44" t="inlineStr">
@@ -2005,7 +2005,7 @@
       <c r="D20" s="47" t="n"/>
       <c r="E20" s="4" t="n"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="30.6" r="21" s="12">
+    <row r="21" ht="30.6" customFormat="1" customHeight="1" s="12">
       <c r="A21" s="43" t="n"/>
       <c r="B21" s="43" t="n"/>
       <c r="C21" s="46" t="n"/>
@@ -2015,14 +2015,14 @@
     <row r="22">
       <c r="E22" s="4" t="n"/>
     </row>
-    <row customHeight="1" ht="28.95" r="23" s="49">
+    <row r="23" ht="28.95" customHeight="1" s="49">
       <c r="A23" s="48" t="inlineStr">
         <is>
           <t>Table 2: List names as last name, first name, middle initial, for whom a personal, family, or business relationship would otherwise preclude their service as a reviewer.</t>
         </is>
       </c>
     </row>
-    <row customFormat="1" r="24" s="9">
+    <row r="24" customFormat="1" s="9">
       <c r="A24" s="56" t="inlineStr">
         <is>
           <t>R:</t>
@@ -2045,7 +2045,7 @@
       </c>
       <c r="E25" s="3" t="n"/>
     </row>
-    <row customFormat="1" r="26" s="9">
+    <row r="26" customFormat="1" s="9">
       <c r="A26" s="13" t="inlineStr">
         <is>
           <t>2</t>
@@ -2072,7 +2072,7 @@
         </is>
       </c>
     </row>
-    <row customFormat="1" r="27" s="9">
+    <row r="27" customFormat="1" s="9">
       <c r="A27" s="19" t="inlineStr">
         <is>
           <t>R:</t>
@@ -2091,42 +2091,42 @@
       <c r="D27" s="20" t="n"/>
       <c r="E27" s="21" t="n"/>
     </row>
-    <row customFormat="1" r="28" s="9">
+    <row r="28" customFormat="1" s="9">
       <c r="A28" s="22" t="n"/>
       <c r="B28" s="20" t="n"/>
       <c r="C28" s="23" t="n"/>
       <c r="D28" s="20" t="n"/>
       <c r="E28" s="21" t="n"/>
     </row>
-    <row customFormat="1" r="29" s="9">
+    <row r="29" customFormat="1" s="9">
       <c r="A29" s="34" t="n"/>
       <c r="B29" s="35" t="n"/>
       <c r="C29" s="35" t="n"/>
       <c r="D29" s="36" t="n"/>
       <c r="E29" s="37" t="n"/>
     </row>
-    <row customFormat="1" r="30" s="9">
+    <row r="30" customFormat="1" s="9">
       <c r="A30" s="34" t="n"/>
       <c r="B30" s="35" t="n"/>
       <c r="C30" s="35" t="n"/>
       <c r="D30" s="36" t="n"/>
       <c r="E30" s="37" t="n"/>
     </row>
-    <row customFormat="1" r="31" s="9">
+    <row r="31" customFormat="1" s="9">
       <c r="A31" s="34" t="n"/>
       <c r="B31" s="35" t="n"/>
       <c r="C31" s="35" t="n"/>
       <c r="D31" s="36" t="n"/>
       <c r="E31" s="37" t="n"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="30.6" r="32" s="9">
+    <row r="32" ht="30.6" customFormat="1" customHeight="1" s="9">
       <c r="A32" s="17" t="n"/>
       <c r="B32" s="18" t="n"/>
       <c r="C32" s="18" t="n"/>
       <c r="D32" s="18" t="n"/>
       <c r="E32" s="4" t="n"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="28.95" r="33" s="9">
+    <row r="33" ht="28.95" customFormat="1" customHeight="1" s="9">
       <c r="A33" s="48" t="inlineStr">
         <is>
           <t>Table 3: List names as last name, first name, middle initial, and provide organizational affiliations, if known, for the following.</t>
@@ -2222,51 +2222,51 @@
       <c r="C39" s="20" t="n"/>
       <c r="D39" s="33" t="n"/>
     </row>
-    <row customFormat="1" r="40" s="9">
+    <row r="40" customFormat="1" s="9">
       <c r="A40" s="19" t="n"/>
       <c r="B40" s="20" t="n"/>
       <c r="C40" s="20" t="n"/>
       <c r="D40" s="32" t="n"/>
     </row>
-    <row customFormat="1" r="41" s="9">
+    <row r="41" customFormat="1" s="9">
       <c r="A41" s="19" t="n"/>
       <c r="B41" s="20" t="n"/>
       <c r="C41" s="20" t="n"/>
       <c r="D41" s="32" t="n"/>
     </row>
-    <row customFormat="1" r="42" s="9">
+    <row r="42" customFormat="1" s="9">
       <c r="A42" s="19" t="n"/>
       <c r="B42" s="35" t="n"/>
       <c r="C42" s="35" t="n"/>
       <c r="D42" s="36" t="n"/>
     </row>
-    <row customFormat="1" r="43" s="9">
+    <row r="43" customFormat="1" s="9">
       <c r="A43" s="19" t="n"/>
       <c r="B43" s="35" t="n"/>
       <c r="C43" s="35" t="n"/>
       <c r="D43" s="36" t="n"/>
     </row>
-    <row customFormat="1" r="44" s="9">
+    <row r="44" customFormat="1" s="9">
       <c r="A44" s="19" t="n"/>
       <c r="B44" s="35" t="n"/>
       <c r="C44" s="35" t="n"/>
       <c r="D44" s="36" t="n"/>
     </row>
-    <row customFormat="1" r="45" s="56">
+    <row r="45" customFormat="1" s="56">
       <c r="A45" s="9" t="n"/>
       <c r="B45" s="9" t="n"/>
       <c r="C45" s="9" t="n"/>
       <c r="D45" s="9" t="n"/>
       <c r="E45" s="4" t="n"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="28.35" r="46" s="56">
+    <row r="46" ht="28.35" customFormat="1" customHeight="1" s="56">
       <c r="A46" s="48" t="inlineStr">
         <is>
           <t>Table 4: List names as last name, first name, middle initial, and provide organizational affiliations, if known, for the following:</t>
         </is>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="27" r="47" s="56">
+    <row r="47" ht="27" customFormat="1" customHeight="1" s="56">
       <c r="A47" s="11" t="inlineStr">
         <is>
           <t>A:</t>
@@ -2304,7 +2304,7 @@
       </c>
       <c r="E49" s="3" t="n"/>
     </row>
-    <row customFormat="1" r="50" s="9">
+    <row r="50" customFormat="1" s="9">
       <c r="A50" s="13" t="inlineStr">
         <is>
           <t>4</t>
@@ -2331,7 +2331,7 @@
         </is>
       </c>
     </row>
-    <row customFormat="1" r="51" s="9">
+    <row r="51" customFormat="1" s="9">
       <c r="A51" s="57" t="inlineStr">
         <is>
           <t>A:</t>
@@ -2350,28 +2350,28 @@
       <c r="D51" s="57" t="n"/>
       <c r="E51" s="57" t="n"/>
     </row>
-    <row customFormat="1" r="52" s="9">
+    <row r="52" customFormat="1" s="9">
       <c r="A52" s="30" t="n"/>
       <c r="B52" s="39" t="n"/>
       <c r="C52" s="39" t="n"/>
       <c r="D52" s="39" t="n"/>
       <c r="E52" s="31" t="n"/>
     </row>
-    <row customFormat="1" r="53" s="9">
+    <row r="53" customFormat="1" s="9">
       <c r="A53" s="9" t="n"/>
       <c r="B53" s="9" t="n"/>
       <c r="C53" s="9" t="n"/>
       <c r="D53" s="9" t="n"/>
       <c r="E53" s="9" t="n"/>
     </row>
-    <row customFormat="1" r="54" s="9">
+    <row r="54" customFormat="1" s="9">
       <c r="A54" s="48" t="inlineStr">
         <is>
           <t>Table 5: List editorial board, editor-in chief and co-editors with whom the individual interacts.  An editor-in-chief must list the entire editorial board.</t>
         </is>
       </c>
     </row>
-    <row customFormat="1" r="55" s="9">
+    <row r="55" customFormat="1" s="9">
       <c r="A55" s="56" t="inlineStr">
         <is>
           <t>B:</t>
@@ -2384,7 +2384,7 @@
       </c>
       <c r="E55" s="3" t="n"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="16.95" r="56" s="56">
+    <row r="56" ht="16.95" customFormat="1" customHeight="1" s="56">
       <c r="A56" s="56" t="inlineStr">
         <is>
           <t>E:</t>
@@ -2397,7 +2397,7 @@
       </c>
       <c r="E56" s="3" t="n"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="28.95" r="57" s="56">
+    <row r="57" ht="28.95" customFormat="1" customHeight="1" s="56">
       <c r="A57" s="56" t="n"/>
       <c r="B57" s="56" t="n"/>
       <c r="C57" s="56" t="n"/>
@@ -2408,7 +2408,7 @@
       </c>
       <c r="E57" s="3" t="n"/>
     </row>
-    <row customFormat="1" r="58" s="56">
+    <row r="58" customFormat="1" s="56">
       <c r="A58" s="13" t="inlineStr">
         <is>
           <t>5</t>
@@ -2435,7 +2435,7 @@
         </is>
       </c>
     </row>
-    <row customFormat="1" r="59" s="56">
+    <row r="59" customFormat="1" s="56">
       <c r="A59" s="19" t="inlineStr">
         <is>
           <t>B:</t>
@@ -2460,7 +2460,7 @@
         <v>42736</v>
       </c>
     </row>
-    <row customFormat="1" r="60" s="9">
+    <row r="60" customFormat="1" s="9">
       <c r="A60" s="22" t="inlineStr">
         <is>
           <t>E:</t>
@@ -2471,28 +2471,28 @@
       <c r="D60" s="20" t="n"/>
       <c r="E60" s="21" t="n"/>
     </row>
-    <row customFormat="1" r="61" s="9">
+    <row r="61" customFormat="1" s="9">
       <c r="A61" s="22" t="n"/>
       <c r="B61" s="23" t="n"/>
       <c r="C61" s="23" t="n"/>
       <c r="D61" s="28" t="n"/>
       <c r="E61" s="21" t="n"/>
     </row>
-    <row customFormat="1" r="62" s="9">
+    <row r="62" customFormat="1" s="9">
       <c r="A62" s="22" t="n"/>
       <c r="B62" s="23" t="n"/>
       <c r="C62" s="23" t="n"/>
       <c r="D62" s="28" t="n"/>
       <c r="E62" s="21" t="n"/>
     </row>
-    <row customFormat="1" r="63" s="9">
+    <row r="63" customFormat="1" s="9">
       <c r="A63" s="24" t="n"/>
       <c r="B63" s="25" t="n"/>
       <c r="C63" s="25" t="n"/>
       <c r="D63" s="26" t="n"/>
       <c r="E63" s="27" t="n"/>
     </row>
-    <row customFormat="1" r="64" s="9"/>
+    <row r="64" customFormat="1" s="9"/>
     <row r="65"/>
     <row r="66"/>
   </sheetData>
@@ -2521,27 +2521,27 @@
     <mergeCell ref="B24:E24"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="A51:A55" type="list">
+    <dataValidation sqref="A51:A55" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"A:,C:"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="A27:A31" type="list">
+    <dataValidation sqref="A27:A31" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"R:"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="A32" type="list">
+    <dataValidation sqref="A32" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"G:,T:,P:"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="A62:A66" type="list">
+    <dataValidation sqref="A62:A66" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"B:,E:"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="0" showErrorMessage="1" showInputMessage="1" sqref="A38:A44" type="list">
+    <dataValidation sqref="A38:A44" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"G:,T:"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink display="https://www.nsf.gov/bfa/dias/policy/coa.jsp" ref="A1" r:id="rId1"/>
+    <hyperlink ref="A1" display="https://www.nsf.gov/bfa/dias/policy/coa.jsp" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup fitToHeight="0" orientation="portrait" scale="98"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" scale="98" fitToHeight="0"/>
   <tableParts count="5">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>

</xml_diff>